<commit_message>
Author: Rashi dhaka file added:rashi dhaka.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/rashi dhaka.xlsx
+++ b/TeamDetails/TasksBreakDown/rashi dhaka.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidhi mishra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashi Dhaka N\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Name 1" sheetId="1" r:id="rId1"/>
@@ -2735,7 +2735,7 @@
   <dimension ref="A2:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,7 +2775,9 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>19</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2785,7 +2787,9 @@
       <c r="E3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
@@ -2800,12 +2804,12 @@
         <v>12</v>
       </c>
       <c r="E4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G46" si="0">E4-F4</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2818,12 +2822,12 @@
         <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>